<commit_message>
Move scripts and notebooks to src and split into three blog parts
</commit_message>
<xml_diff>
--- a/Data/EindeStemperiode.xlsx
+++ b/Data/EindeStemperiode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\Willekeurige berekeningen\Top2000\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63279F-088B-411C-A46F-C242D7EF0BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E951E8F-3818-4A60-BDEC-82D5CE99CF24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="3285" windowWidth="18900" windowHeight="11055" xr2:uid="{752754DA-EEEB-4E92-B295-2A0DFA45B989}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{752754DA-EEEB-4E92-B295-2A0DFA45B989}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>http://www.40u.radio.nl/48158/top-2000-stemperiode-trekt-5-miljoen-luisteraars</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>JaarTop2000</t>
+  </si>
+  <si>
+    <t>https://www.parool.nl/nieuws/veel-animo-voor-stemmen-op-top-2000~b743b9a8/</t>
+  </si>
+  <si>
+    <t>https://www.radiofreak.nl/stemmen-voor-top-2000-begint-morgen/</t>
+  </si>
+  <si>
+    <t>https://www.radiofreak.nl/stemming-voor-radio-2-top-2000-begonnen/</t>
+  </si>
+  <si>
+    <t>https://www.radiofreak.nl/radio-2-start-maandag-met-de-top-2000/</t>
   </si>
 </sst>
 </file>
@@ -415,7 +427,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +550,9 @@
       <c r="B13">
         <v>2009</v>
       </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -569,60 +584,81 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>38687</v>
+        <v>38686</v>
       </c>
       <c r="B17">
         <v>2005</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>38322</v>
+        <v>38331</v>
       </c>
       <c r="B18">
         <v>2004</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>37956</v>
+        <v>37970</v>
       </c>
       <c r="B19">
         <v>2003</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>37591</v>
       </c>
       <c r="B20">
         <v>2002</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>37226</v>
       </c>
       <c r="B21">
         <v>2001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>36861</v>
       </c>
       <c r="B22">
         <v>2000</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>36495</v>
       </c>
       <c r="B23">
         <v>1999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>